<commit_message>
Updated Auther for excel, now it will show my name.
</commit_message>
<xml_diff>
--- a/doc/distrib/Samples/Data/helix.xlsx
+++ b/doc/distrib/Samples/Data/helix.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="315" windowWidth="18855" windowHeight="11715"/>
@@ -13,13 +13,9 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -547,6 +543,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -625,6 +626,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -659,6 +661,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -834,16 +837,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0.3517846</v>
       </c>
@@ -854,7 +857,7 @@
         <v>-2.8734790000000001</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.50576339999999997</v>
       </c>
@@ -865,7 +868,7 @@
         <v>-2.871073</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.64226130000000003</v>
       </c>
@@ -876,7 +879,7 @@
         <v>-2.8685999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.75547989999999998</v>
       </c>
@@ -887,7 +890,7 @@
         <v>-2.8660559999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.84043769999999995</v>
       </c>
@@ -898,7 +901,7 @@
         <v>-2.8634400000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.89319000000000004</v>
       </c>
@@ -909,7 +912,7 @@
         <v>-2.8607480000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.9110007</v>
       </c>
@@ -920,7 +923,7 @@
         <v>-2.8579780000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.89247759999999998</v>
       </c>
@@ -931,7 +934,7 @@
         <v>-2.8551259999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.83765089999999998</v>
       </c>
@@ -942,7 +945,7 @@
         <v>-2.8521899999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.74800250000000001</v>
       </c>
@@ -953,7 +956,7 @@
         <v>-2.8491650000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.62643150000000003</v>
       </c>
@@ -964,7 +967,7 @@
         <v>-2.84605</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0.47717120000000002</v>
       </c>
@@ -975,7 +978,7 @@
         <v>-2.8428390000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0.30564720000000001</v>
       </c>
@@ -986,7 +989,7 @@
         <v>-2.8395299999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0.1182791</v>
       </c>
@@ -997,7 +1000,7 @@
         <v>-2.8361190000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>-7.7742464999999997E-2</v>
       </c>
@@ -1008,7 +1011,7 @@
         <v>-2.8326009999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>-0.27473969999999998</v>
       </c>
@@ -1019,7 +1022,7 @@
         <v>-2.8289710000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>-0.46482970000000001</v>
       </c>
@@ -1030,7 +1033,7 @@
         <v>-2.8252259999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>-0.64023909999999995</v>
       </c>
@@ -1041,7 +1044,7 @@
         <v>-2.8213599999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>-0.79361990000000004</v>
       </c>
@@ -1052,7 +1055,7 @@
         <v>-2.8173680000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>-0.91833949999999998</v>
       </c>
@@ -1063,7 +1066,7 @@
         <v>-2.8132459999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>-1.0087699999999999</v>
       </c>
@@ -1074,7 +1077,7 @@
         <v>-2.8089879999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>-1.0605249999999999</v>
       </c>
@@ -1085,7 +1088,7 @@
         <v>-2.804586</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>-1.070667</v>
       </c>
@@ -1096,7 +1099,7 @@
         <v>-2.8000370000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>-1.037852</v>
       </c>
@@ -1107,7 +1110,7 @@
         <v>-2.7953320000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>-0.96242090000000002</v>
       </c>
@@ -1118,7 +1121,7 @@
         <v>-2.7904659999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>-0.84642300000000004</v>
       </c>
@@ -1129,7 +1132,7 @@
         <v>-2.7854299999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>-0.69357340000000001</v>
       </c>
@@ -1140,7 +1143,7 @@
         <v>-2.7802180000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>-0.50914380000000004</v>
       </c>
@@ -1151,7 +1154,7 @@
         <v>-2.7748210000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>-0.29978880000000002</v>
       </c>
@@ -1162,7 +1165,7 @@
         <v>-2.769231</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>-7.3318548999999997E-2</v>
       </c>
@@ -1173,7 +1176,7 @@
         <v>-2.763439</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0.16159029999999999</v>
       </c>
@@ -1184,7 +1187,7 @@
         <v>-2.7574350000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>0.39571339999999999</v>
       </c>
@@ -1195,7 +1198,7 @@
         <v>-2.7512099999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>0.61963250000000003</v>
       </c>
@@ -1206,7 +1209,7 @@
         <v>-2.7447530000000002</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>0.82410519999999998</v>
       </c>
@@ -1217,7 +1220,7 @@
         <v>-2.738054</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1.000432</v>
       </c>
@@ -1228,7 +1231,7 @@
         <v>-2.7311000000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1.140819</v>
       </c>
@@ -1239,7 +1242,7 @@
         <v>-2.723878</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1.2387090000000001</v>
       </c>
@@ -1250,7 +1253,7 @@
         <v>-2.716377</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1.2890710000000001</v>
       </c>
@@ -1261,7 +1264,7 @@
         <v>-2.7085810000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1.28864</v>
       </c>
@@ -1272,7 +1275,7 @@
         <v>-2.7004779999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1.236092</v>
       </c>
@@ -1283,7 +1286,7 @@
         <v>-2.6920500000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1.1321490000000001</v>
       </c>
@@ -1294,7 +1297,7 @@
         <v>-2.683281</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>0.97960100000000006</v>
       </c>
@@ -1305,7 +1308,7 @@
         <v>-2.6741549999999998</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>0.78325619999999996</v>
       </c>
@@ -1316,7 +1319,7 @@
         <v>-2.6646529999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>0.54980039999999997</v>
       </c>
@@ -1327,7 +1330,7 @@
         <v>-2.6547540000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>0.2875895</v>
       </c>
@@ -1338,7 +1341,7 @@
         <v>-2.6444399999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>6.3577644000000003E-3</v>
       </c>
@@ -1349,7 +1352,7 @@
         <v>-2.6336870000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>-0.2831245</v>
       </c>
@@ -1360,7 +1363,7 @@
         <v>-2.6224720000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>-0.56945009999999996</v>
       </c>
@@ -1371,7 +1374,7 @@
         <v>-2.61077</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>-0.84100969999999997</v>
       </c>
@@ -1382,7 +1385,7 @@
         <v>-2.598557</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>-1.086441</v>
       </c>
@@ -1393,7 +1396,7 @@
         <v>-2.5858029999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>-1.295096</v>
       </c>
@@ -1404,7 +1407,7 @@
         <v>-2.572479</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>-1.4574769999999999</v>
       </c>
@@ -1415,7 +1418,7 @@
         <v>-2.558554</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>-1.56565</v>
       </c>
@@ -1426,7 +1429,7 @@
         <v>-2.5439949999999998</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>-1.6136109999999999</v>
       </c>
@@ -1437,7 +1440,7 @@
         <v>-2.5287660000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>-1.597577</v>
       </c>
@@ -1448,7 +1451,7 @@
         <v>-2.512832</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>-1.5162119999999999</v>
       </c>
@@ -1459,7 +1462,7 @@
         <v>-2.4961509999999998</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>-1.3707560000000001</v>
       </c>
@@ -1470,7 +1473,7 @@
         <v>-2.4786820000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>-1.165054</v>
       </c>
@@ -1481,7 +1484,7 @@
         <v>-2.4603809999999999</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>-0.90549060000000003</v>
       </c>
@@ -1492,7 +1495,7 @@
         <v>-2.4411999999999998</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>-0.60082270000000004</v>
       </c>
@@ -1503,7 +1506,7 @@
         <v>-2.4210910000000001</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>-0.26190010000000002</v>
       </c>
@@ -1514,7 +1517,7 @@
         <v>-2.4</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>9.8691246999999996E-2</v>
       </c>
@@ -1525,7 +1528,7 @@
         <v>-2.377872</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>0.46707530000000003</v>
       </c>
@@ -1536,7 +1539,7 @@
         <v>-2.3546480000000001</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>0.82859369999999999</v>
       </c>
@@ -1547,7 +1550,7 @@
         <v>-2.3302670000000001</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>1.168371</v>
       </c>
@@ -1558,7 +1561,7 @@
         <v>-2.3046639999999998</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>1.4718990000000001</v>
       </c>
@@ -1569,7 +1572,7 @@
         <v>-2.2777699999999999</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>1.7256359999999999</v>
       </c>
@@ -1580,7 +1583,7 @@
         <v>-2.249514</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>1.9175869999999999</v>
       </c>
@@ -1591,7 +1594,7 @@
         <v>-2.2198199999999999</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2.0378400000000001</v>
       </c>
@@ -1602,7 +1605,7 @@
         <v>-2.188612</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2.0790500000000001</v>
       </c>
@@ -1613,7 +1616,7 @@
         <v>-2.1558060000000001</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2.036829</v>
       </c>
@@ -1624,7 +1627,7 @@
         <v>-2.1213199999999999</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>1.9100349999999999</v>
       </c>
@@ -1635,7 +1638,7 @@
         <v>-2.0850659999999999</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>1.700944</v>
       </c>
@@ -1646,7 +1649,7 @@
         <v>-2.0469550000000001</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>1.4152910000000001</v>
       </c>
@@ -1657,7 +1660,7 @@
         <v>-2.006894</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>1.0621579999999999</v>
       </c>
@@ -1668,7 +1671,7 @@
         <v>-1.9647920000000001</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>0.65374600000000005</v>
       </c>
@@ -1679,7 +1682,7 @@
         <v>-1.920553</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>0.20497609999999999</v>
       </c>
@@ -1690,7 +1693,7 @@
         <v>-1.874085</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>-0.26701510000000001</v>
       </c>
@@ -1701,7 +1704,7 @@
         <v>-1.8252949999999999</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>-0.7435041</v>
       </c>
@@ -1712,7 +1715,7 @@
         <v>-1.7740910000000001</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>-1.204912</v>
       </c>
@@ -1723,7 +1726,7 @@
         <v>-1.7203870000000001</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>-1.6315930000000001</v>
       </c>
@@ -1734,7 +1737,7 @@
         <v>-1.6641010000000001</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>-2.0046740000000001</v>
       </c>
@@ -1745,7 +1748,7 @@
         <v>-1.605156</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>-2.3068919999999999</v>
       </c>
@@ -1756,7 +1759,7 @@
         <v>-1.5434870000000001</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>-2.5234079999999999</v>
       </c>
@@ -1767,7 +1770,7 @@
         <v>-1.4790380000000001</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>-2.6425450000000001</v>
       </c>
@@ -1778,7 +1781,7 @@
         <v>-1.4117649999999999</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>-2.6564290000000002</v>
       </c>
@@ -1789,7 +1792,7 @@
         <v>-1.3416410000000001</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>-2.5614780000000001</v>
       </c>
@@ -1800,7 +1803,7 @@
         <v>-1.268656</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>-2.3587289999999999</v>
       </c>
@@ -1811,7 +1814,7 @@
         <v>-1.192822</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>-2.0539589999999999</v>
       </c>
@@ -1822,7 +1825,7 @@
         <v>-1.1141719999999999</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>-1.657589</v>
       </c>
@@ -1833,7 +1836,7 @@
         <v>-1.032764</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>-1.184375</v>
       </c>
@@ -1844,7 +1847,7 @@
         <v>-0.94868330000000001</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>-0.65286029999999995</v>
       </c>
@@ -1855,7 +1858,7 @@
         <v>-0.86204369999999997</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>-8.4640867999999994E-2</v>
       </c>
@@ -1866,7 +1869,7 @@
         <v>-0.77298800000000001</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>0.49656309999999998</v>
       </c>
@@ -1877,7 +1880,7 @@
         <v>-0.68168890000000004</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>1.065963</v>
       </c>
@@ -1888,7 +1891,7 @@
         <v>-0.58834839999999999</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>1.5988530000000001</v>
       </c>
@@ -1899,7 +1902,7 @@
         <v>-0.493197</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2.0717850000000002</v>
       </c>
@@ -1910,7 +1913,7 @@
         <v>-0.39649119999999999</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>2.4637190000000002</v>
       </c>
@@ -1921,7 +1924,7 @@
         <v>-0.29851109999999997</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2.757063</v>
       </c>
@@ -1932,7 +1935,7 @@
         <v>-0.19955709999999999</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>2.9385680000000001</v>
       </c>
@@ -1943,7 +1946,7 @@
         <v>-9.9944494999999994E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>3</v>
       </c>
@@ -1954,7 +1957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>2.9385680000000001</v>
       </c>
@@ -1965,7 +1968,7 @@
         <v>9.9944494999999994E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>2.757063</v>
       </c>
@@ -1976,7 +1979,7 @@
         <v>0.19955709999999999</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>2.4637190000000002</v>
       </c>
@@ -1987,7 +1990,7 @@
         <v>0.29851109999999997</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>2.0717850000000002</v>
       </c>
@@ -1998,7 +2001,7 @@
         <v>0.39649119999999999</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>1.5988530000000001</v>
       </c>
@@ -2009,7 +2012,7 @@
         <v>0.493197</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>1.065963</v>
       </c>
@@ -2020,7 +2023,7 @@
         <v>0.58834839999999999</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>0.49656309999999998</v>
       </c>
@@ -2031,7 +2034,7 @@
         <v>0.68168890000000004</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>-8.4640867999999994E-2</v>
       </c>
@@ -2042,7 +2045,7 @@
         <v>0.77298800000000001</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>-0.65286029999999995</v>
       </c>
@@ -2053,7 +2056,7 @@
         <v>0.86204369999999997</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>-1.184375</v>
       </c>
@@ -2064,7 +2067,7 @@
         <v>0.94868330000000001</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>-1.657589</v>
       </c>
@@ -2075,7 +2078,7 @@
         <v>1.032764</v>
       </c>
     </row>
-    <row r="113" spans="1:3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>-2.0539589999999999</v>
       </c>
@@ -2086,7 +2089,7 @@
         <v>1.1141719999999999</v>
       </c>
     </row>
-    <row r="114" spans="1:3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>-2.3587289999999999</v>
       </c>
@@ -2097,7 +2100,7 @@
         <v>1.192822</v>
       </c>
     </row>
-    <row r="115" spans="1:3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>-2.5614780000000001</v>
       </c>
@@ -2108,7 +2111,7 @@
         <v>1.268656</v>
       </c>
     </row>
-    <row r="116" spans="1:3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>-2.6564290000000002</v>
       </c>
@@ -2119,7 +2122,7 @@
         <v>1.3416410000000001</v>
       </c>
     </row>
-    <row r="117" spans="1:3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>-2.6425450000000001</v>
       </c>
@@ -2130,7 +2133,7 @@
         <v>1.4117649999999999</v>
       </c>
     </row>
-    <row r="118" spans="1:3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>-2.5234079999999999</v>
       </c>
@@ -2141,7 +2144,7 @@
         <v>1.4790380000000001</v>
       </c>
     </row>
-    <row r="119" spans="1:3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>-2.3068919999999999</v>
       </c>
@@ -2152,7 +2155,7 @@
         <v>1.5434870000000001</v>
       </c>
     </row>
-    <row r="120" spans="1:3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>-2.0046740000000001</v>
       </c>
@@ -2163,7 +2166,7 @@
         <v>1.605156</v>
       </c>
     </row>
-    <row r="121" spans="1:3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>-1.6315930000000001</v>
       </c>
@@ -2174,7 +2177,7 @@
         <v>1.6641010000000001</v>
       </c>
     </row>
-    <row r="122" spans="1:3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>-1.204912</v>
       </c>
@@ -2185,7 +2188,7 @@
         <v>1.7203870000000001</v>
       </c>
     </row>
-    <row r="123" spans="1:3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>-0.7435041</v>
       </c>
@@ -2196,7 +2199,7 @@
         <v>1.7740910000000001</v>
       </c>
     </row>
-    <row r="124" spans="1:3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>-0.26701510000000001</v>
       </c>
@@ -2207,7 +2210,7 @@
         <v>1.8252949999999999</v>
       </c>
     </row>
-    <row r="125" spans="1:3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>0.20497609999999999</v>
       </c>
@@ -2218,7 +2221,7 @@
         <v>1.874085</v>
       </c>
     </row>
-    <row r="126" spans="1:3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>0.65374600000000005</v>
       </c>
@@ -2229,7 +2232,7 @@
         <v>1.920553</v>
       </c>
     </row>
-    <row r="127" spans="1:3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>1.0621579999999999</v>
       </c>
@@ -2240,7 +2243,7 @@
         <v>1.9647920000000001</v>
       </c>
     </row>
-    <row r="128" spans="1:3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>1.4152910000000001</v>
       </c>
@@ -2251,7 +2254,7 @@
         <v>2.006894</v>
       </c>
     </row>
-    <row r="129" spans="1:3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>1.700944</v>
       </c>
@@ -2262,7 +2265,7 @@
         <v>2.0469550000000001</v>
       </c>
     </row>
-    <row r="130" spans="1:3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>1.9100349999999999</v>
       </c>
@@ -2273,7 +2276,7 @@
         <v>2.0850659999999999</v>
       </c>
     </row>
-    <row r="131" spans="1:3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>2.036829</v>
       </c>
@@ -2284,7 +2287,7 @@
         <v>2.1213199999999999</v>
       </c>
     </row>
-    <row r="132" spans="1:3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>2.0790500000000001</v>
       </c>
@@ -2295,7 +2298,7 @@
         <v>2.1558060000000001</v>
       </c>
     </row>
-    <row r="133" spans="1:3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>2.0378400000000001</v>
       </c>
@@ -2306,7 +2309,7 @@
         <v>2.188612</v>
       </c>
     </row>
-    <row r="134" spans="1:3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>1.9175869999999999</v>
       </c>
@@ -2317,7 +2320,7 @@
         <v>2.2198199999999999</v>
       </c>
     </row>
-    <row r="135" spans="1:3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>1.7256359999999999</v>
       </c>
@@ -2328,7 +2331,7 @@
         <v>2.249514</v>
       </c>
     </row>
-    <row r="136" spans="1:3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>1.4718990000000001</v>
       </c>
@@ -2339,7 +2342,7 @@
         <v>2.2777699999999999</v>
       </c>
     </row>
-    <row r="137" spans="1:3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>1.168371</v>
       </c>
@@ -2350,7 +2353,7 @@
         <v>2.3046639999999998</v>
       </c>
     </row>
-    <row r="138" spans="1:3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>0.82859369999999999</v>
       </c>
@@ -2361,7 +2364,7 @@
         <v>2.3302670000000001</v>
       </c>
     </row>
-    <row r="139" spans="1:3">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>0.46707530000000003</v>
       </c>
@@ -2372,7 +2375,7 @@
         <v>2.3546480000000001</v>
       </c>
     </row>
-    <row r="140" spans="1:3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>9.8691246999999996E-2</v>
       </c>
@@ -2383,7 +2386,7 @@
         <v>2.377872</v>
       </c>
     </row>
-    <row r="141" spans="1:3">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>-0.26190010000000002</v>
       </c>
@@ -2394,7 +2397,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="142" spans="1:3">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>-0.60082270000000004</v>
       </c>
@@ -2405,7 +2408,7 @@
         <v>2.4210910000000001</v>
       </c>
     </row>
-    <row r="143" spans="1:3">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>-0.90549060000000003</v>
       </c>
@@ -2416,7 +2419,7 @@
         <v>2.4411999999999998</v>
       </c>
     </row>
-    <row r="144" spans="1:3">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>-1.165054</v>
       </c>
@@ -2427,7 +2430,7 @@
         <v>2.4603809999999999</v>
       </c>
     </row>
-    <row r="145" spans="1:3">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>-1.3707560000000001</v>
       </c>
@@ -2438,7 +2441,7 @@
         <v>2.4786820000000001</v>
       </c>
     </row>
-    <row r="146" spans="1:3">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>-1.5162119999999999</v>
       </c>
@@ -2449,7 +2452,7 @@
         <v>2.4961509999999998</v>
       </c>
     </row>
-    <row r="147" spans="1:3">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>-1.597577</v>
       </c>
@@ -2460,7 +2463,7 @@
         <v>2.512832</v>
       </c>
     </row>
-    <row r="148" spans="1:3">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>-1.6136109999999999</v>
       </c>
@@ -2471,7 +2474,7 @@
         <v>2.5287660000000001</v>
       </c>
     </row>
-    <row r="149" spans="1:3">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>-1.56565</v>
       </c>
@@ -2482,7 +2485,7 @@
         <v>2.5439949999999998</v>
       </c>
     </row>
-    <row r="150" spans="1:3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>-1.4574769999999999</v>
       </c>
@@ -2493,7 +2496,7 @@
         <v>2.558554</v>
       </c>
     </row>
-    <row r="151" spans="1:3">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>-1.295096</v>
       </c>
@@ -2504,7 +2507,7 @@
         <v>2.572479</v>
       </c>
     </row>
-    <row r="152" spans="1:3">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>-1.086441</v>
       </c>
@@ -2515,7 +2518,7 @@
         <v>2.5858029999999999</v>
       </c>
     </row>
-    <row r="153" spans="1:3">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>-0.84100969999999997</v>
       </c>
@@ -2526,7 +2529,7 @@
         <v>2.598557</v>
       </c>
     </row>
-    <row r="154" spans="1:3">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>-0.56945009999999996</v>
       </c>
@@ -2537,7 +2540,7 @@
         <v>2.61077</v>
       </c>
     </row>
-    <row r="155" spans="1:3">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>-0.2831245</v>
       </c>
@@ -2548,7 +2551,7 @@
         <v>2.6224720000000001</v>
       </c>
     </row>
-    <row r="156" spans="1:3">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>6.3577644000000003E-3</v>
       </c>
@@ -2559,7 +2562,7 @@
         <v>2.6336870000000001</v>
       </c>
     </row>
-    <row r="157" spans="1:3">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>0.2875895</v>
       </c>
@@ -2570,7 +2573,7 @@
         <v>2.6444399999999999</v>
       </c>
     </row>
-    <row r="158" spans="1:3">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>0.54980039999999997</v>
       </c>
@@ -2581,7 +2584,7 @@
         <v>2.6547540000000001</v>
       </c>
     </row>
-    <row r="159" spans="1:3">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>0.78325619999999996</v>
       </c>
@@ -2592,7 +2595,7 @@
         <v>2.6646529999999999</v>
       </c>
     </row>
-    <row r="160" spans="1:3">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>0.97960100000000006</v>
       </c>
@@ -2603,7 +2606,7 @@
         <v>2.6741549999999998</v>
       </c>
     </row>
-    <row r="161" spans="1:3">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>1.1321490000000001</v>
       </c>
@@ -2614,7 +2617,7 @@
         <v>2.683281</v>
       </c>
     </row>
-    <row r="162" spans="1:3">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>1.236092</v>
       </c>
@@ -2625,7 +2628,7 @@
         <v>2.6920500000000001</v>
       </c>
     </row>
-    <row r="163" spans="1:3">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>1.28864</v>
       </c>
@@ -2636,7 +2639,7 @@
         <v>2.7004779999999999</v>
       </c>
     </row>
-    <row r="164" spans="1:3">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>1.2890710000000001</v>
       </c>
@@ -2647,7 +2650,7 @@
         <v>2.7085810000000001</v>
       </c>
     </row>
-    <row r="165" spans="1:3">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>1.2387090000000001</v>
       </c>
@@ -2658,7 +2661,7 @@
         <v>2.716377</v>
       </c>
     </row>
-    <row r="166" spans="1:3">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>1.140819</v>
       </c>
@@ -2669,7 +2672,7 @@
         <v>2.723878</v>
       </c>
     </row>
-    <row r="167" spans="1:3">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>1.000432</v>
       </c>
@@ -2680,7 +2683,7 @@
         <v>2.7311000000000001</v>
       </c>
     </row>
-    <row r="168" spans="1:3">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>0.82410519999999998</v>
       </c>
@@ -2691,7 +2694,7 @@
         <v>2.738054</v>
       </c>
     </row>
-    <row r="169" spans="1:3">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>0.61963250000000003</v>
       </c>
@@ -2702,7 +2705,7 @@
         <v>2.7447530000000002</v>
       </c>
     </row>
-    <row r="170" spans="1:3">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>0.39571339999999999</v>
       </c>
@@ -2713,7 +2716,7 @@
         <v>2.7512099999999999</v>
       </c>
     </row>
-    <row r="171" spans="1:3">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>0.16159029999999999</v>
       </c>
@@ -2724,7 +2727,7 @@
         <v>2.7574350000000001</v>
       </c>
     </row>
-    <row r="172" spans="1:3">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>-7.3318548999999997E-2</v>
       </c>
@@ -2735,7 +2738,7 @@
         <v>2.763439</v>
       </c>
     </row>
-    <row r="173" spans="1:3">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>-0.29978880000000002</v>
       </c>
@@ -2746,7 +2749,7 @@
         <v>2.769231</v>
       </c>
     </row>
-    <row r="174" spans="1:3">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>-0.50914380000000004</v>
       </c>
@@ -2757,7 +2760,7 @@
         <v>2.7748210000000002</v>
       </c>
     </row>
-    <row r="175" spans="1:3">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>-0.69357340000000001</v>
       </c>
@@ -2768,7 +2771,7 @@
         <v>2.7802180000000001</v>
       </c>
     </row>
-    <row r="176" spans="1:3">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>-0.84642300000000004</v>
       </c>
@@ -2779,7 +2782,7 @@
         <v>2.7854299999999999</v>
       </c>
     </row>
-    <row r="177" spans="1:3">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>-0.96242090000000002</v>
       </c>
@@ -2790,7 +2793,7 @@
         <v>2.7904659999999999</v>
       </c>
     </row>
-    <row r="178" spans="1:3">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>-1.037852</v>
       </c>
@@ -2801,7 +2804,7 @@
         <v>2.7953320000000001</v>
       </c>
     </row>
-    <row r="179" spans="1:3">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>-1.070667</v>
       </c>
@@ -2812,7 +2815,7 @@
         <v>2.8000370000000001</v>
       </c>
     </row>
-    <row r="180" spans="1:3">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>-1.0605249999999999</v>
       </c>
@@ -2823,7 +2826,7 @@
         <v>2.804586</v>
       </c>
     </row>
-    <row r="181" spans="1:3">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>-1.0087699999999999</v>
       </c>
@@ -2834,7 +2837,7 @@
         <v>2.8089879999999998</v>
       </c>
     </row>
-    <row r="182" spans="1:3">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>-0.91833949999999998</v>
       </c>
@@ -2845,7 +2848,7 @@
         <v>2.8132459999999999</v>
       </c>
     </row>
-    <row r="183" spans="1:3">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>-0.79361990000000004</v>
       </c>
@@ -2856,7 +2859,7 @@
         <v>2.8173680000000001</v>
       </c>
     </row>
-    <row r="184" spans="1:3">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>-0.64023909999999995</v>
       </c>
@@ -2867,7 +2870,7 @@
         <v>2.8213599999999999</v>
       </c>
     </row>
-    <row r="185" spans="1:3">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>-0.46482970000000001</v>
       </c>
@@ -2878,7 +2881,7 @@
         <v>2.8252259999999998</v>
       </c>
     </row>
-    <row r="186" spans="1:3">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>-0.27473969999999998</v>
       </c>
@@ -2889,7 +2892,7 @@
         <v>2.8289710000000001</v>
       </c>
     </row>
-    <row r="187" spans="1:3">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>-7.7742464999999997E-2</v>
       </c>
@@ -2900,7 +2903,7 @@
         <v>2.8326009999999999</v>
       </c>
     </row>
-    <row r="188" spans="1:3">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>0.1182791</v>
       </c>
@@ -2911,7 +2914,7 @@
         <v>2.8361190000000001</v>
       </c>
     </row>
-    <row r="189" spans="1:3">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>0.30564720000000001</v>
       </c>
@@ -2922,7 +2925,7 @@
         <v>2.8395299999999999</v>
       </c>
     </row>
-    <row r="190" spans="1:3">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>0.47717120000000002</v>
       </c>
@@ -2933,7 +2936,7 @@
         <v>2.8428390000000001</v>
       </c>
     </row>
-    <row r="191" spans="1:3">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>0.62643150000000003</v>
       </c>
@@ -2944,7 +2947,7 @@
         <v>2.84605</v>
       </c>
     </row>
-    <row r="192" spans="1:3">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>0.74800250000000001</v>
       </c>
@@ -2955,7 +2958,7 @@
         <v>2.8491650000000002</v>
       </c>
     </row>
-    <row r="193" spans="1:3">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>0.83765089999999998</v>
       </c>
@@ -2966,7 +2969,7 @@
         <v>2.8521899999999998</v>
       </c>
     </row>
-    <row r="194" spans="1:3">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>0.89247759999999998</v>
       </c>
@@ -2977,7 +2980,7 @@
         <v>2.8551259999999998</v>
       </c>
     </row>
-    <row r="195" spans="1:3">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>0.9110007</v>
       </c>
@@ -2988,7 +2991,7 @@
         <v>2.8579780000000001</v>
       </c>
     </row>
-    <row r="196" spans="1:3">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>0.89319000000000004</v>
       </c>
@@ -2999,7 +3002,7 @@
         <v>2.8607480000000001</v>
       </c>
     </row>
-    <row r="197" spans="1:3">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>0.84043769999999995</v>
       </c>
@@ -3010,7 +3013,7 @@
         <v>2.8634400000000002</v>
       </c>
     </row>
-    <row r="198" spans="1:3">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>0.75547989999999998</v>
       </c>
@@ -3021,7 +3024,7 @@
         <v>2.8660559999999999</v>
       </c>
     </row>
-    <row r="199" spans="1:3">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>0.64226130000000003</v>
       </c>
@@ -3032,7 +3035,7 @@
         <v>2.8685999999999998</v>
       </c>
     </row>
-    <row r="200" spans="1:3">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>0.50576339999999997</v>
       </c>
@@ -3043,7 +3046,7 @@
         <v>2.871073</v>
       </c>
     </row>
-    <row r="201" spans="1:3">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>0.3517846</v>
       </c>

</xml_diff>